<commit_message>
update .csv files with conflicts resolved. Add the kappa statistic results from the second training set to analyses/03
</commit_message>
<xml_diff>
--- a/outputs/scopingSearchSummary.xlsx
+++ b/outputs/scopingSearchSummary.xlsx
@@ -1,21 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deviv\R-working-folder\OBS_systematic_map\outputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Search.Formula</t>
+  </si>
+  <si>
+    <t>N_total_results</t>
+  </si>
+  <si>
+    <t>N_test_list</t>
+  </si>
+  <si>
+    <t>N_percent_test_list</t>
+  </si>
+  <si>
+    <t>(OCEAN_RELATED) AND (OCEAN_RENEWABLE) NOT (NO_TERMS)</t>
+  </si>
+  <si>
+    <t>(OCEAN_RELATED) AND (CLIMATE_CHANGE) NOT (NO_TERMS)</t>
+  </si>
+  <si>
+    <t>(OCEAN_RELATED) AND ((CLIMATE_CHANGE) AND ((OPTION) NEAR/5 (MIT_ADAPT))) NOT (NO_TERMS)</t>
+  </si>
+  <si>
+    <t>(OCEAN_RELATED) AND (CLIMATE_CHANGE) AND (INTERVENTION_MIT) NOT (NO_TERMS)</t>
+  </si>
+  <si>
+    <t>(OCEAN_RELATED) AND (CLIMATE_CHANGE) AND (INTERVENTION_NAT) NOT (NO_TERMS)</t>
+  </si>
+  <si>
+    <t>(OCEAN_RELATED) AND (CLIMATE_CHANGE) AND (SOC_ADAPT) AND ((INTERVENTION_SA_BIT) OR (INTERVENTION_SA_SOC_INST)) NOT (NO_TERMS)</t>
+  </si>
+  <si>
+    <t>(OCEAN_RELATED) AND ((OCEAN_RENEWABLE) OR ((CLIMATE_CHANGE) AND ((OPTION) NEAR/5 (MIT_ADAPT))) OR ((CLIMATE_CHANGE) AND ((INTERVENTION_MIT) OR (INTERVENTION_NAT) OR ((SOC_ADAPT) AND ((INTERVENTION_SA_BIT) OR (INTERVENTION_SA_SOC_INST)))))) NOT (NO_TERMS)</t>
+  </si>
+  <si>
+    <t>Add (pollution OR pollutant$) to NOT terms</t>
+  </si>
+  <si>
+    <t>Search_No</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,10 +101,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -63,11 +121,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +207,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +242,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,160 +418,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="138.1796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Search.Formula</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>N_total_results</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>N_test_list</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>N_percent_test_list</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>(OCEAN_RELATED) AND (OCEAN_RENEWABLE) NOT (NO_TERMS)</t>
-        </is>
-      </c>
-      <c r="B2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
         <v>42555</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>18</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>18.55670103092784</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>(OCEAN_RELATED) AND (CLIMATE_CHANGE) NOT (NO_TERMS)</t>
-        </is>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>498888</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>89</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>91.75257731958763</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>(OCEAN_RELATED) AND ((CLIMATE_CHANGE) AND ((OPTION) NEAR/5 (MIT_ADAPT))) NOT (NO_TERMS)</t>
-        </is>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
         <v>13869</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>29</v>
       </c>
-      <c r="D4">
-        <v>29.89690721649485</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>(OCEAN_RELATED) AND (CLIMATE_CHANGE) AND (INTERVENTION_MIT) NOT (NO_TERMS)</t>
-        </is>
-      </c>
-      <c r="B5">
+      <c r="E4">
+        <v>29.896907216494849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>152368</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>50</v>
       </c>
-      <c r="D5">
-        <v>51.54639175257731</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>(OCEAN_RELATED) AND (CLIMATE_CHANGE) AND (INTERVENTION_NAT) NOT (NO_TERMS)</t>
-        </is>
-      </c>
-      <c r="B6">
+      <c r="E5">
+        <v>51.546391752577307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
         <v>163312</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>72</v>
       </c>
-      <c r="D6">
-        <v>74.22680412371135</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>(OCEAN_RELATED) AND (CLIMATE_CHANGE) AND (SOC_ADAPT) AND ((INTERVENTION_SA_BIT) OR (INTERVENTION_SA_SOC_INST)) NOT (NO_TERMS)</t>
-        </is>
-      </c>
-      <c r="B7">
+      <c r="E6">
+        <v>74.226804123711347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
         <v>10138</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>29</v>
       </c>
-      <c r="D7">
-        <v>29.89690721649485</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>(OCEAN_RELATED) AND ((OCEAN_RENEWABLE) OR ((CLIMATE_CHANGE) AND ((OPTION) NEAR/5 (MIT_ADAPT))) OR ((CLIMATE_CHANGE) AND ((INTERVENTION_MIT) OR (INTERVENTION_NAT) OR ((SOC_ADAPT) AND ((INTERVENTION_SA_BIT) OR (INTERVENTION_SA_SOC_INST)))))) NOT (NO_TERMS)</t>
-        </is>
-      </c>
-      <c r="B8">
+      <c r="E7">
+        <v>29.896907216494849</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
         <v>292256</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>97</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>100</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Add (pollution OR pollutant$) to NOT terms</t>
-        </is>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
         <v>277012</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>95</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>97.9381443298969</v>
       </c>
     </row>

</xml_diff>